<commit_message>
Ya no funciona getSublist
</commit_message>
<xml_diff>
--- a/productos.xlsx
+++ b/productos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10043042\Documents\IntelliJProjects\ReadExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E67B50-5679-4306-AE88-93B0176488B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0E2E3F-B99B-41DA-BA6D-129A3E9F0ABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18825" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Codigo</t>
   </si>
@@ -52,13 +52,31 @@
   </si>
   <si>
     <t>Pepitas</t>
+  </si>
+  <si>
+    <t>CGWVHQB</t>
+  </si>
+  <si>
+    <t>MVRBVIWB</t>
+  </si>
+  <si>
+    <t>SUYWGFW</t>
+  </si>
+  <si>
+    <t>PEIOJECKJ</t>
+  </si>
+  <si>
+    <t>WHBVWKDJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +97,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -97,22 +120,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,12 +421,12 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
@@ -406,86 +434,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>8.5</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>10</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>8.5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>4.5</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>10</v>
       </c>
     </row>

</xml_diff>